<commit_message>
fix: fixed composite title generation
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/Словники.xlsx
+++ b/renderer/dictionaries/Словники.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8A6BB1-2082-BE43-9FE6-A2AB6748498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B77624C-8712-E844-ADF9-251C2993853F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{18F3DDB0-F3B0-4042-A2E8-682B46F64E38}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
   <si>
     <t>старший науковий співробітник</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>Назва посади в давальному відмінку</t>
+  </si>
+  <si>
+    <t>Прізвище в давальному відмінку</t>
   </si>
 </sst>
 </file>
@@ -929,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2E3F80-3793-CA4E-A0A1-B472298AB53B}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -971,7 +974,7 @@
         <v>87</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
fix:fixed title index storing in temp_book
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/Словники.xlsx
+++ b/renderer/dictionaries/Словники.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E1AF7D-EEC7-0B45-B88D-7613D94F24A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776404A8-8CCD-2543-9236-BB601E25FA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
   <si>
     <t>Ідентифікатор</t>
   </si>
@@ -64,15 +64,6 @@
     <t>начальника служби</t>
   </si>
   <si>
-    <t>діловод</t>
-  </si>
-  <si>
-    <t>діловоду</t>
-  </si>
-  <si>
-    <t>діловода</t>
-  </si>
-  <si>
     <t>Назва підрозділу в називному відмінку</t>
   </si>
   <si>
@@ -121,18 +112,6 @@
     <t>служб</t>
   </si>
   <si>
-    <t>штаб</t>
-  </si>
-  <si>
-    <t>штабу</t>
-  </si>
-  <si>
-    <t>відділ персоналу та стройового</t>
-  </si>
-  <si>
-    <t>відділу персоналу та стройового</t>
-  </si>
-  <si>
     <t>Ім'я та по батькові в називному відмінку</t>
   </si>
   <si>
@@ -260,6 +239,9 @@
   </si>
   <si>
     <t>юстиції</t>
+  </si>
+  <si>
+    <t>990390</t>
   </si>
   <si>
     <t>так</t>
@@ -746,9 +728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -808,33 +792,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -843,13 +815,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -857,10 +829,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -871,13 +843,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -885,10 +857,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -899,10 +871,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -913,13 +885,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -927,47 +899,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D9" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -977,7 +921,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,61 +931,61 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="O1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="P1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Q1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1049,40 +993,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1091,19 +1035,19 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1111,40 +1055,40 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J3" t="s">
         <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" t="s">
-        <v>72</v>
       </c>
       <c r="K3">
         <v>5</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="N3">
         <v>4</v>
@@ -1156,16 +1100,16 @@
         <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="S3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="T3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1173,40 +1117,40 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K4">
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N4">
         <v>5</v>
@@ -1221,16 +1165,19 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="S4" t="s">
+        <v>72</v>
       </c>
       <c r="T4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:T3 A4:R4 T4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:T4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1245,10 +1192,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1256,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1264,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1272,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1280,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1288,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1296,7 +1243,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1304,7 +1251,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1312,7 +1259,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1320,7 +1267,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1328,7 +1275,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1336,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1344,7 +1291,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1352,7 +1299,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1360,7 +1307,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1368,7 +1315,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1376,7 +1323,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1384,7 +1331,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1392,7 +1339,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1400,7 +1347,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1408,7 +1355,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1416,7 +1363,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1424,7 +1371,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1432,7 +1379,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1440,7 +1387,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1448,7 +1395,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1456,7 +1403,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1464,7 +1411,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1472,7 +1419,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1480,7 +1427,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1488,7 +1435,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1496,7 +1443,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1504,7 +1451,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1512,7 +1459,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1520,7 +1467,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1528,7 +1475,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1536,7 +1483,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1544,7 +1491,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1552,7 +1499,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1560,7 +1507,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1568,7 +1515,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1576,7 +1523,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1584,7 +1531,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:transited to title indexes
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/Словники.xlsx
+++ b/renderer/dictionaries/Словники.xlsx
@@ -1,40 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776404A8-8CCD-2543-9236-BB601E25FA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4081346-D02F-3B4B-8D75-19EAF2D22FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Посади" sheetId="1" r:id="rId1"/>
+    <sheet name="Ролі" sheetId="1" r:id="rId1"/>
     <sheet name="Підрозділи" sheetId="2" r:id="rId2"/>
-    <sheet name="Персонал" sheetId="3" r:id="rId3"/>
-    <sheet name="Військові звання" sheetId="4" r:id="rId4"/>
+    <sheet name="Посади" sheetId="3" r:id="rId3"/>
+    <sheet name="Персонал" sheetId="4" r:id="rId4"/>
+    <sheet name="Військові звання" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="155">
   <si>
     <t>Ідентифікатор</t>
   </si>
   <si>
-    <t>Назва посади в називному відмінку</t>
-  </si>
-  <si>
-    <t>Назва посади в давальному відмінку</t>
-  </si>
-  <si>
-    <t>Назва посади в знахідному відмінку</t>
+    <t>Назва ролі в називному відмінку</t>
+  </si>
+  <si>
+    <t>Назва ролі в давальному відмінку</t>
+  </si>
+  <si>
+    <t>Назва ролі в знахідному відмінку</t>
   </si>
   <si>
     <t>старший науковий співробітник</t>
@@ -46,6 +47,15 @@
     <t>старшого наукового співробітника</t>
   </si>
   <si>
+    <t>дідовод</t>
+  </si>
+  <si>
+    <t>дідоводу</t>
+  </si>
+  <si>
+    <t>дідовода</t>
+  </si>
+  <si>
     <t>водій - електрик</t>
   </si>
   <si>
@@ -112,6 +122,18 @@
     <t>служб</t>
   </si>
   <si>
+    <t>Індекс посади</t>
+  </si>
+  <si>
+    <t>Основна роль (ідентифікатор з аркуша "Ролі")</t>
+  </si>
+  <si>
+    <t>Основний підрозділ (ідентифікатор з аркуша "Підрозділи")</t>
+  </si>
+  <si>
+    <t>Вторинний підрозділ (ідентифікатор з аркуша "Підрозділи")</t>
+  </si>
+  <si>
     <t>Ім'я та по батькові в називному відмінку</t>
   </si>
   <si>
@@ -148,24 +170,9 @@
     <t>Гендер</t>
   </si>
   <si>
-    <t>Основна посада (ідентифікатор з аркуша "Посади")</t>
-  </si>
-  <si>
-    <t>Основний підрозділ (ідентифікатор з аркуша "Підрозділи")</t>
-  </si>
-  <si>
-    <t>Вторинна посада (через тире до основної посади, ідентифікатор з аркуша "Посади")</t>
-  </si>
-  <si>
-    <t>Вторинний підрозділ (ідентифікатор з аркуша "Підрозділи")</t>
-  </si>
-  <si>
     <t>На котловому забезпеченні при...</t>
   </si>
   <si>
-    <t>Індекс посади</t>
-  </si>
-  <si>
     <t>Звільнений/переведений</t>
   </si>
   <si>
@@ -196,6 +203,9 @@
     <t>військовій частині A0000</t>
   </si>
   <si>
+    <t>000001</t>
+  </si>
+  <si>
     <t>Олена Ігорівна</t>
   </si>
   <si>
@@ -229,7 +239,7 @@
     <t>Міністерстві оборони України</t>
   </si>
   <si>
-    <t>0012003</t>
+    <t>000002</t>
   </si>
   <si>
     <t>І.К.</t>
@@ -247,6 +257,105 @@
     <t>так</t>
   </si>
   <si>
+    <t>Перш Першович</t>
+  </si>
+  <si>
+    <t>Перша Першовича</t>
+  </si>
+  <si>
+    <t>Першу Першовичу</t>
+  </si>
+  <si>
+    <t>П.П.</t>
+  </si>
+  <si>
+    <t>ПЕРШИЙ</t>
+  </si>
+  <si>
+    <t>ПЕРШОГО</t>
+  </si>
+  <si>
+    <t>ПЕРШОМУ</t>
+  </si>
+  <si>
+    <t>вічі 1100</t>
+  </si>
+  <si>
+    <t>111000</t>
+  </si>
+  <si>
+    <t>ні</t>
+  </si>
+  <si>
+    <t>Друг Другич</t>
+  </si>
+  <si>
+    <t>Друга Другича</t>
+  </si>
+  <si>
+    <t>Другу Другичу</t>
+  </si>
+  <si>
+    <t>Д.Д.</t>
+  </si>
+  <si>
+    <t>ДРУГИЙ</t>
+  </si>
+  <si>
+    <t>ДРУГОГО</t>
+  </si>
+  <si>
+    <t>ДРУГОМУ</t>
+  </si>
+  <si>
+    <t>вічі 2211</t>
+  </si>
+  <si>
+    <t>222000</t>
+  </si>
+  <si>
+    <t>ТРЕТ ТРЕТІЧ</t>
+  </si>
+  <si>
+    <t>ТРЕТЯ ТРЕТІЧА</t>
+  </si>
+  <si>
+    <t>ТРЕТЮ ТРЕТІЧУ</t>
+  </si>
+  <si>
+    <t>Т.Т.</t>
+  </si>
+  <si>
+    <t>ТРЕТІЙ</t>
+  </si>
+  <si>
+    <t>ТРЕТЬОГО</t>
+  </si>
+  <si>
+    <t>ТРЕТЬОМУ</t>
+  </si>
+  <si>
+    <t>вічі 3424</t>
+  </si>
+  <si>
+    <t>333000</t>
+  </si>
+  <si>
+    <t>Ч.Ч.</t>
+  </si>
+  <si>
+    <t>ЧЕТВЕРТИЙ</t>
+  </si>
+  <si>
+    <t>ЧЕТВЕРТОГО</t>
+  </si>
+  <si>
+    <t>вічі 4455</t>
+  </si>
+  <si>
+    <t>444000</t>
+  </si>
+  <si>
     <t>Відповідник "rank" аркуша "Військовослужбовці"</t>
   </si>
   <si>
@@ -377,6 +486,9 @@
   </si>
   <si>
     <t>адмірал</t>
+  </si>
+  <si>
+    <t>Вторинна роль (через тире до основної ролі, ідентифікатор з аркуша "Ролі")</t>
   </si>
 </sst>
 </file>
@@ -728,11 +840,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -766,7 +876,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -780,7 +890,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -790,12 +900,26 @@
       </c>
       <c r="D4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -804,9 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -815,13 +937,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -829,10 +951,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -843,13 +965,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -857,10 +979,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -871,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -885,13 +1007,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -899,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -918,272 +1040,584 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
+        <v>71</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3">
-        <v>5</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3">
-        <v>4</v>
-      </c>
-      <c r="O3">
-        <v>6</v>
-      </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" t="s">
-        <v>68</v>
-      </c>
-      <c r="T3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-      <c r="L4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="O4">
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="P4">
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="Q4">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" t="s">
-        <v>72</v>
-      </c>
-      <c r="T4" t="s">
-        <v>73</v>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:T4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D1 A2:A4 C2:E4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6" t="s">
+        <v>95</v>
+      </c>
+      <c r="P6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O7" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>108</v>
+      </c>
+      <c r="O8" t="s">
+        <v>109</v>
+      </c>
+      <c r="P8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:P8" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1192,10 +1626,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1203,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1211,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1219,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1227,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1235,7 +1669,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1243,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1251,7 +1685,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,7 +1693,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1267,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1275,7 +1709,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1283,7 +1717,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1291,7 +1725,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1299,7 +1733,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1307,7 +1741,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1315,7 +1749,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1323,7 +1757,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1331,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1339,7 +1773,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1347,7 +1781,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1355,7 +1789,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1363,7 +1797,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1371,7 +1805,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1379,7 +1813,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1387,7 +1821,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1395,7 +1829,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1403,7 +1837,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1411,7 +1845,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1419,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1427,7 +1861,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1435,7 +1869,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1443,7 +1877,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1451,7 +1885,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1459,7 +1893,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1467,7 +1901,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1475,7 +1909,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1483,7 +1917,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1491,7 +1925,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1499,7 +1933,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1507,7 +1941,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1515,7 +1949,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1523,7 +1957,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1531,7 +1965,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added assigning new servants along with saving to dictionary
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/Словники.xlsx
+++ b/renderer/dictionaries/Словники.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4081346-D02F-3B4B-8D75-19EAF2D22FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258CBD3E-EF21-B649-B998-3AEE81575FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ролі" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="163">
   <si>
     <t>Ідентифікатор</t>
   </si>
@@ -131,9 +131,33 @@
     <t>Основний підрозділ (ідентифікатор з аркуша "Підрозділи")</t>
   </si>
   <si>
+    <t>Вторинна роль (через тире до основної ролі, ідентифікатор з аркуша "Ролі")</t>
+  </si>
+  <si>
     <t>Вторинний підрозділ (ідентифікатор з аркуша "Підрозділи")</t>
   </si>
   <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>000002</t>
+  </si>
+  <si>
+    <t>990390</t>
+  </si>
+  <si>
+    <t>111000</t>
+  </si>
+  <si>
+    <t>222000</t>
+  </si>
+  <si>
+    <t>333000</t>
+  </si>
+  <si>
+    <t>444000</t>
+  </si>
+  <si>
     <t>Ім'я та по батькові в називному відмінку</t>
   </si>
   <si>
@@ -203,9 +227,6 @@
     <t>військовій частині A0000</t>
   </si>
   <si>
-    <t>000001</t>
-  </si>
-  <si>
     <t>Олена Ігорівна</t>
   </si>
   <si>
@@ -239,9 +260,6 @@
     <t>Міністерстві оборони України</t>
   </si>
   <si>
-    <t>000002</t>
-  </si>
-  <si>
     <t>І.К.</t>
   </si>
   <si>
@@ -251,9 +269,6 @@
     <t>юстиції</t>
   </si>
   <si>
-    <t>990390</t>
-  </si>
-  <si>
     <t>так</t>
   </si>
   <si>
@@ -281,9 +296,6 @@
     <t>вічі 1100</t>
   </si>
   <si>
-    <t>111000</t>
-  </si>
-  <si>
     <t>ні</t>
   </si>
   <si>
@@ -311,9 +323,6 @@
     <t>вічі 2211</t>
   </si>
   <si>
-    <t>222000</t>
-  </si>
-  <si>
     <t>ТРЕТ ТРЕТІЧ</t>
   </si>
   <si>
@@ -338,9 +347,6 @@
     <t>вічі 3424</t>
   </si>
   <si>
-    <t>333000</t>
-  </si>
-  <si>
     <t>Ч.Ч.</t>
   </si>
   <si>
@@ -353,7 +359,28 @@
     <t>вічі 4455</t>
   </si>
   <si>
-    <t>444000</t>
+    <t>Пят Пятич</t>
+  </si>
+  <si>
+    <t>Пята Пятича</t>
+  </si>
+  <si>
+    <t>Пяту Пятичу</t>
+  </si>
+  <si>
+    <t>ПЯТАКА</t>
+  </si>
+  <si>
+    <t>ПЯТАКИ</t>
+  </si>
+  <si>
+    <t>ПЯТАЦІ</t>
+  </si>
+  <si>
+    <t>ПЯТАКУ</t>
+  </si>
+  <si>
+    <t>вічі 0055</t>
   </si>
   <si>
     <t>Відповідник "rank" аркуша "Військовослужбовці"</t>
@@ -486,9 +513,6 @@
   </si>
   <si>
     <t>адмірал</t>
-  </si>
-  <si>
-    <t>Вторинна роль (через тире до основної ролі, ідентифікатор з аркуша "Ролі")</t>
   </si>
 </sst>
 </file>
@@ -1042,9 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1062,10 +1084,10 @@
         <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1073,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1090,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1107,7 +1129,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1124,7 +1146,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1138,7 +1160,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1158,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1178,7 +1200,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1193,17 +1215,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D1 A2:A4 C2:E4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1213,49 +1235,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="M1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="N1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="O1" t="s">
         <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1263,31 +1285,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1296,13 +1318,13 @@
         <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="P2" t="s">
         <v>23</v>
@@ -1313,31 +1335,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -1346,13 +1368,13 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="N3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s">
         <v>23</v>
@@ -1375,10 +1397,10 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
         <v>23</v>
@@ -1393,7 +1415,7 @@
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M4" t="s">
         <v>23</v>
@@ -1402,10 +1424,10 @@
         <v>23</v>
       </c>
       <c r="O4" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -1413,31 +1435,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="K5">
         <v>6</v>
@@ -1449,13 +1471,13 @@
         <v>23</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="O5" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -1463,31 +1485,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="K6">
         <v>19</v>
@@ -1499,13 +1521,13 @@
         <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O6" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="P6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -1513,31 +1535,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K7">
         <v>27</v>
@@ -1549,13 +1571,13 @@
         <v>23</v>
       </c>
       <c r="N7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O7" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="P7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1575,10 +1597,10 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
@@ -1587,7 +1609,7 @@
         <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K8">
         <v>7</v>
@@ -1599,19 +1621,69 @@
         <v>23</v>
       </c>
       <c r="N8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="O8" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="P8" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9">
+        <v>29</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" t="s">
+        <v>118</v>
+      </c>
+      <c r="O9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:P8" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:P9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1626,10 +1698,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1637,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1645,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1653,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1661,7 +1733,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1669,7 +1741,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1677,7 +1749,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1685,7 +1757,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1693,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1701,7 +1773,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1709,7 +1781,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1717,7 +1789,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1725,7 +1797,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1733,7 +1805,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1741,7 +1813,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1749,7 +1821,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1757,7 +1829,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1765,7 +1837,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1773,7 +1845,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1781,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1789,7 +1861,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1797,7 +1869,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1805,7 +1877,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1813,7 +1885,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1821,7 +1893,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1829,7 +1901,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1837,7 +1909,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1845,7 +1917,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1853,7 +1925,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1861,7 +1933,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1869,7 +1941,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1877,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1885,7 +1957,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1893,7 +1965,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1901,7 +1973,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1909,7 +1981,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1917,7 +1989,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1925,7 +1997,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1933,7 +2005,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1941,7 +2013,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1949,7 +2021,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1957,7 +2029,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1965,7 +2037,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added personnel reassignment page
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/Словники.xlsx
+++ b/renderer/dictionaries/Словники.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258CBD3E-EF21-B649-B998-3AEE81575FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4F89FF-C03F-9F4C-B1D2-3438D6819511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ролі" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="168">
   <si>
     <t>Ідентифікатор</t>
   </si>
@@ -513,6 +513,21 @@
   </si>
   <si>
     <t>адмірал</t>
+  </si>
+  <si>
+    <t>Назва ролі в орудному відмінку</t>
+  </si>
+  <si>
+    <t>старшим науковим співробітником</t>
+  </si>
+  <si>
+    <t>дідоводом</t>
+  </si>
+  <si>
+    <t>водієм - електриком</t>
+  </si>
+  <si>
+    <t>начальником служби</t>
   </si>
 </sst>
 </file>
@@ -864,13 +879,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -883,8 +900,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -897,8 +917,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -911,8 +934,11 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -925,8 +951,11 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -938,6 +967,9 @@
       </c>
       <c r="D5" t="s">
         <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat:added contract page to personnel orders
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/Словники.xlsx
+++ b/renderer/dictionaries/Словники.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4F89FF-C03F-9F4C-B1D2-3438D6819511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D47A08-D70B-8A41-B0FC-010B02283B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ролі" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="187">
   <si>
     <t>Ідентифікатор</t>
   </si>
@@ -38,6 +38,9 @@
     <t>Назва ролі в знахідному відмінку</t>
   </si>
   <si>
+    <t>Назва ролі в орудному відмінку</t>
+  </si>
+  <si>
     <t>старший науковий співробітник</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t>старшого наукового співробітника</t>
   </si>
   <si>
+    <t>старшим науковим співробітником</t>
+  </si>
+  <si>
     <t>дідовод</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
     <t>дідовода</t>
   </si>
   <si>
+    <t>дідоводом</t>
+  </si>
+  <si>
     <t>водій - електрик</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
     <t>водія - електрика</t>
   </si>
   <si>
+    <t>водієм - електриком</t>
+  </si>
+  <si>
     <t>начальник служби</t>
   </si>
   <si>
@@ -74,6 +86,21 @@
     <t>начальника служби</t>
   </si>
   <si>
+    <t>начальником служби</t>
+  </si>
+  <si>
+    <t>камікадзе</t>
+  </si>
+  <si>
+    <t>камікадзі</t>
+  </si>
+  <si>
+    <t>камікадзу</t>
+  </si>
+  <si>
+    <t>камікадзей</t>
+  </si>
+  <si>
     <t>Назва підрозділу в називному відмінку</t>
   </si>
   <si>
@@ -515,19 +542,49 @@
     <t>адмірал</t>
   </si>
   <si>
-    <t>Назва ролі в орудному відмінку</t>
-  </si>
-  <si>
-    <t>старшим науковим співробітником</t>
-  </si>
-  <si>
-    <t>дідоводом</t>
-  </si>
-  <si>
-    <t>водієм - електриком</t>
-  </si>
-  <si>
-    <t>начальником служби</t>
+    <t>Прізвище в орудному відмінку</t>
+  </si>
+  <si>
+    <t>Ім'я та по батькові в орудному відмінку</t>
+  </si>
+  <si>
+    <t>Василем Сергійовичем</t>
+  </si>
+  <si>
+    <t>Оленою Ігорівною</t>
+  </si>
+  <si>
+    <t>Першем Першовичем</t>
+  </si>
+  <si>
+    <t>Другом Другичем</t>
+  </si>
+  <si>
+    <t>ТРЕТЄМ ТРЕТІЧЕМ</t>
+  </si>
+  <si>
+    <t>Пятом Пятичем</t>
+  </si>
+  <si>
+    <t>ІВАНОВИМ</t>
+  </si>
+  <si>
+    <t>ГРАБОВОЮ</t>
+  </si>
+  <si>
+    <t>ПЕРШИМ</t>
+  </si>
+  <si>
+    <t>ДРУГИМ</t>
+  </si>
+  <si>
+    <t>ТРЕТІМ</t>
+  </si>
+  <si>
+    <t>ЧЕТВЕРТИМ</t>
+  </si>
+  <si>
+    <t>ПЯТАКОМ</t>
   </si>
 </sst>
 </file>
@@ -879,11 +936,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -901,7 +956,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>163</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -909,16 +964,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>164</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -926,16 +981,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -943,16 +998,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -960,22 +1015,39 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -993,13 +1065,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1007,10 +1079,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1021,13 +1093,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1035,10 +1107,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -1049,10 +1121,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1063,13 +1135,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1077,13 +1149,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1107,19 +1179,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1127,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1136,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1144,7 +1216,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1153,7 +1225,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1161,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1178,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1192,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1212,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1232,7 +1304,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1254,468 +1326,522 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>173</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="L1" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="N1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="P1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>174</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2">
+        <v>73</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>65</v>
-      </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3">
+        <v>83</v>
+      </c>
+      <c r="K3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M3">
         <v>5</v>
       </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>76</v>
-      </c>
       <c r="N3" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
-      </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="O4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="P4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="J5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5">
         <v>6</v>
       </c>
-      <c r="L5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" t="s">
-        <v>23</v>
-      </c>
       <c r="N5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="O5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6">
+        <v>106</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" t="s">
+        <v>183</v>
+      </c>
+      <c r="M6">
         <v>19</v>
       </c>
-      <c r="L6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" t="s">
-        <v>23</v>
-      </c>
       <c r="N6" t="s">
-        <v>98</v>
+        <v>32</v>
       </c>
       <c r="O6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="P6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L7" t="s">
+        <v>184</v>
+      </c>
+      <c r="M7">
+        <v>27</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" t="s">
         <v>99</v>
       </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7">
-        <v>27</v>
-      </c>
-      <c r="L7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8">
+        <v>32</v>
+      </c>
+      <c r="K8" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="s">
-        <v>23</v>
-      </c>
       <c r="N8" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="O8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="P8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>179</v>
       </c>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="I9" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="J9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K9">
+        <v>125</v>
+      </c>
+      <c r="K9" t="s">
+        <v>126</v>
+      </c>
+      <c r="L9" t="s">
+        <v>186</v>
+      </c>
+      <c r="M9">
         <v>29</v>
       </c>
-      <c r="L9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" t="s">
-        <v>65</v>
-      </c>
       <c r="N9" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="O9" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="P9" t="s">
-        <v>90</v>
+        <v>127</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:P9" numberStoredAsText="1"/>
+    <ignoredError sqref="M1:R9 A1:E9 G1:K9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1730,10 +1856,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1741,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1749,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1757,7 +1883,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1765,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1773,7 +1899,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1781,7 +1907,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1789,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1797,7 +1923,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1805,7 +1931,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1813,7 +1939,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1821,7 +1947,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1829,7 +1955,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1837,7 +1963,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1845,7 +1971,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1853,7 +1979,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1861,7 +1987,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1869,7 +1995,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1877,7 +2003,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1885,7 +2011,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1893,7 +2019,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1901,7 +2027,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1909,7 +2035,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1917,7 +2043,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1925,7 +2051,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1933,7 +2059,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1941,7 +2067,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1949,7 +2075,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1957,7 +2083,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1965,7 +2091,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1973,7 +2099,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1981,7 +2107,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1989,7 +2115,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1997,7 +2123,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2005,7 +2131,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2013,7 +2139,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2021,7 +2147,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2029,7 +2155,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2037,7 +2163,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2045,7 +2171,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2053,7 +2179,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2061,7 +2187,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2069,7 +2195,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>